<commit_message>
Cambios interfaz y codigo backed
</commit_message>
<xml_diff>
--- a/Interfaz/ExcelPrueba.xlsx
+++ b/Interfaz/ExcelPrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Google Drive\WORK\ExcelsStuff\Interfaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8438B9C6-E233-49CD-82FE-F26E262FDB2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98000DC7-AD86-4F66-96F1-E01C5E1BC111}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{13016273-4EF2-4B62-95F6-A43C8078E435}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$47</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="106">
   <si>
     <t>RAT</t>
   </si>
@@ -715,10 +715,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B60EC4D-321C-412B-B796-DB7989863D93}">
-  <dimension ref="A1:Q47"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -829,7 +830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -879,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -929,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1129,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1929,7 +1930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2129,7 +2130,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2276,7 +2277,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -2767,13 +2768,13 @@
         <v>53</v>
       </c>
       <c r="P41">
-        <v>45.757763975155299</v>
+        <v>4</v>
       </c>
       <c r="Q41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>53</v>
       </c>
       <c r="P42">
-        <v>53.4596273291925</v>
+        <v>2</v>
       </c>
       <c r="Q42" t="s">
         <v>98</v>
@@ -2867,13 +2868,13 @@
         <v>53</v>
       </c>
       <c r="P43">
-        <v>61.1614906832298</v>
+        <v>2</v>
       </c>
       <c r="Q43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -2917,13 +2918,13 @@
         <v>53</v>
       </c>
       <c r="P44">
-        <v>68.863354037267101</v>
+        <v>3</v>
       </c>
       <c r="Q44" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>53</v>
       </c>
       <c r="P45">
-        <v>76.565217391304301</v>
+        <v>2</v>
       </c>
       <c r="Q45" t="s">
         <v>101</v>
@@ -3017,7 +3018,7 @@
         <v>53</v>
       </c>
       <c r="P46">
-        <v>84.267080745341602</v>
+        <v>5</v>
       </c>
       <c r="Q46" t="s">
         <v>100</v>
@@ -3064,14 +3065,214 @@
         <v>53</v>
       </c>
       <c r="P47">
-        <v>84.267080745341602</v>
+        <v>2</v>
       </c>
       <c r="Q47" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50">
+        <v>925</v>
+      </c>
+      <c r="E50">
+        <v>6666</v>
+      </c>
+      <c r="F50">
+        <v>667</v>
+      </c>
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" s="4">
+        <v>-113585</v>
+      </c>
+      <c r="I50">
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <v>90</v>
+      </c>
+      <c r="K50" t="s">
+        <v>53</v>
+      </c>
+      <c r="L50" t="s">
+        <v>53</v>
+      </c>
+      <c r="M50" t="s">
+        <v>53</v>
+      </c>
+      <c r="O50" t="s">
+        <v>53</v>
+      </c>
+      <c r="P50">
+        <v>84</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51">
+        <v>925</v>
+      </c>
+      <c r="E51">
+        <v>6666</v>
+      </c>
+      <c r="G51" t="s">
+        <v>70</v>
+      </c>
+      <c r="H51" s="4">
+        <v>-113588</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+      <c r="J51">
+        <v>90</v>
+      </c>
+      <c r="K51" t="s">
+        <v>53</v>
+      </c>
+      <c r="L51" t="s">
+        <v>53</v>
+      </c>
+      <c r="M51" t="s">
+        <v>53</v>
+      </c>
+      <c r="O51" t="s">
+        <v>53</v>
+      </c>
+      <c r="P51">
+        <v>84</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53">
+        <v>925</v>
+      </c>
+      <c r="E53">
+        <v>555</v>
+      </c>
+      <c r="F53">
+        <v>444</v>
+      </c>
+      <c r="G53" t="s">
+        <v>70</v>
+      </c>
+      <c r="H53" s="4">
+        <v>-113585</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>90</v>
+      </c>
+      <c r="K53" t="s">
+        <v>53</v>
+      </c>
+      <c r="L53" t="s">
+        <v>53</v>
+      </c>
+      <c r="M53" t="s">
+        <v>53</v>
+      </c>
+      <c r="O53" t="s">
+        <v>53</v>
+      </c>
+      <c r="P53">
+        <v>84</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54">
+        <v>925</v>
+      </c>
+      <c r="E54">
+        <v>555</v>
+      </c>
+      <c r="G54" t="s">
+        <v>70</v>
+      </c>
+      <c r="H54" s="4">
+        <v>-113588</v>
+      </c>
+      <c r="I54">
+        <v>6</v>
+      </c>
+      <c r="J54">
+        <v>90</v>
+      </c>
+      <c r="K54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L54" t="s">
+        <v>53</v>
+      </c>
+      <c r="M54" t="s">
+        <v>53</v>
+      </c>
+      <c r="O54" t="s">
+        <v>53</v>
+      </c>
+      <c r="P54">
+        <v>84</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{DA3E0645-785D-4B69-939E-4BE12B28FF22}"/>
+  <autoFilter ref="A1:Q47" xr:uid="{61F35A59-DF7C-4D60-AC9A-5E1403AF1B98}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios guardado de archivos
</commit_message>
<xml_diff>
--- a/Interfaz/ExcelPrueba.xlsx
+++ b/Interfaz/ExcelPrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Google Drive\WORK\ExcelsStuff\Interfaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98000DC7-AD86-4F66-96F1-E01C5E1BC111}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1C1E3B-8307-45DC-8A17-12ED1F7402BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{13016273-4EF2-4B62-95F6-A43C8078E435}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$47</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -718,13 +718,14 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambios cantidad de HITS
</commit_message>
<xml_diff>
--- a/Interfaz/ExcelPrueba.xlsx
+++ b/Interfaz/ExcelPrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Google Drive\WORK\ExcelsStuff\Interfaz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D580CD-2B19-425A-89F4-EAD4656F37C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257CD2E2-8515-43F3-A88E-FC7C5FB4CAE9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{13016273-4EF2-4B62-95F6-A43C8078E435}"/>
   </bookViews>
@@ -718,8 +718,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -831,7 +831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -881,7 +881,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -931,7 +931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -981,7 +981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -3314,8 +3314,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q47" xr:uid="{61F35A59-DF7C-4D60-AC9A-5E1403AF1B98}">
-    <filterColumn colId="4">
+  <autoFilter ref="A1:Q47" xr:uid="{AC70FF13-2882-4219-A54D-98E3EEC05EB1}">
+    <filterColumn colId="5">
       <filters>
         <filter val="1"/>
       </filters>

</xml_diff>